<commit_message>
Implement and test adjustment of named tables, ranges and merged cells
</commit_message>
<xml_diff>
--- a/test/templates/test-named-tables.xlsx
+++ b/test/templates/test-named-tables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
@@ -12,6 +12,8 @@
   <definedNames>
     <definedName name="BelowTable">Tables!$B$16</definedName>
     <definedName name="Moving">Tables!$E$7</definedName>
+    <definedName name="RangeBelowTable">Tables!$B$17:$C$17</definedName>
+    <definedName name="RangeRightOfTable">Tables!$E$12:$F$12</definedName>
     <definedName name="RightOfTable">Tables!$D$7</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -133,13 +135,13 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -506,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F16"/>
+  <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F12" sqref="E12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -520,10 +522,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="20" thickBot="1">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="2:6" ht="16" thickTop="1"/>
     <row r="4" spans="2:6">
@@ -552,10 +554,10 @@
       <c r="D7">
         <v>101</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <v>102</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" t="s">
@@ -566,13 +568,13 @@
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="3">
+      <c r="B10" s="4">
         <v>103</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
@@ -580,6 +582,12 @@
       </c>
       <c r="D12" t="s">
         <v>9</v>
+      </c>
+      <c r="E12">
+        <v>107</v>
+      </c>
+      <c r="F12">
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="2:6">
@@ -601,6 +609,14 @@
     <row r="16" spans="2:6">
       <c r="B16">
         <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17">
+        <v>105</v>
+      </c>
+      <c r="C17">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test for totals row on tables
</commit_message>
<xml_diff>
--- a/test/templates/test-named-tables.xlsx
+++ b/test/templates/test-named-tables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Named tables</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>Bad</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -154,11 +160,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Ages" displayName="Ages" ref="B4:C5" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Ages" displayName="Ages" ref="B4:C6" totalsRowCount="1">
   <autoFilter ref="B4:C5"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="Age"/>
+    <tableColumn id="1" name="Name" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Age" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -508,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F17"/>
+  <dimension ref="B2:J27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="E12:F12"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -544,6 +550,15 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="2:6">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <f>SUBTOTAL(103,Ages[Age])</f>
+        <v>1</v>
+      </c>
+    </row>
     <row r="7" spans="2:6">
       <c r="B7" t="s">
         <v>1</v>
@@ -611,12 +626,17 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:10">
       <c r="B17">
         <v>105</v>
       </c>
       <c r="C17">
         <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="J27" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add test for _xlnm.Print_Titles named range
</commit_message>
<xml_diff>
--- a/test/templates/test-named-tables.xlsx
+++ b/test/templates/test-named-tables.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mitrais\cac\olive-2021\xlsx-template\test\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC52F1DE-F66C-4F7A-9A91-F3AAAF458473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -12,12 +18,23 @@
   <definedNames>
     <definedName name="BelowTable">Tables!$B$16</definedName>
     <definedName name="Moving">Tables!$E$7</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Tables!$1:$3</definedName>
     <definedName name="RangeBelowTable">Tables!$B$17:$C$17</definedName>
     <definedName name="RangeRightOfTable">Tables!$E$12:$F$12</definedName>
     <definedName name="RightOfTable">Tables!$D$7</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -82,7 +99,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -156,37 +173,45 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Ages" displayName="Ages" ref="B4:C6" totalsRowCount="1">
-  <autoFilter ref="B4:C5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Ages" displayName="Ages" ref="B4:C6" totalsRowCount="1">
+  <autoFilter ref="B4:C5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Name" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Age" totalsRowFunction="count"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Age" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Days" displayName="Days" ref="B7:C8" totalsRowShown="0">
-  <autoFilter ref="B7:C8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Days" displayName="Days" ref="B7:C8" totalsRowShown="0">
+  <autoFilter ref="B7:C8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="${days}"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="${days}"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Status" displayName="Status" ref="C12:D14" totalsRowShown="0">
-  <autoFilter ref="C12:D14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Status" displayName="Status" ref="C12:D14" totalsRowShown="0">
+  <autoFilter ref="C12:D14" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Colour"/>
-    <tableColumn id="2" name="Status"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Colour"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -513,28 +538,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="20" thickBot="1">
+    <row r="2" spans="2:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="2:6" ht="16" thickTop="1"/>
-    <row r="4" spans="2:6">
+    <row r="3" spans="2:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -542,7 +567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -550,7 +575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -559,7 +584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -574,7 +599,7 @@
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -582,13 +607,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>103</v>
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
@@ -605,7 +630,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>11</v>
       </c>
@@ -613,7 +638,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
@@ -621,12 +646,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>105</v>
       </c>
@@ -634,7 +659,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="2:10">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="J27" t="s">
         <v>16</v>
       </c>
@@ -645,12 +670,12 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="E7:F7"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <tableParts count="3">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Fixing Defined Range Name with Sheet Name (#150)
* fixing defined range name with sheetname
* add test for _xlnm.Print_Titles named range

Co-authored-by: Ade Pangestu <ade.pangestu@mitrais.com>
</commit_message>
<xml_diff>
--- a/test/templates/test-named-tables.xlsx
+++ b/test/templates/test-named-tables.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mitrais\cac\olive-2021\xlsx-template\test\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC52F1DE-F66C-4F7A-9A91-F3AAAF458473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -12,12 +18,23 @@
   <definedNames>
     <definedName name="BelowTable">Tables!$B$16</definedName>
     <definedName name="Moving">Tables!$E$7</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Tables!$1:$3</definedName>
     <definedName name="RangeBelowTable">Tables!$B$17:$C$17</definedName>
     <definedName name="RangeRightOfTable">Tables!$E$12:$F$12</definedName>
     <definedName name="RightOfTable">Tables!$D$7</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -82,7 +99,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -156,37 +173,45 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Ages" displayName="Ages" ref="B4:C6" totalsRowCount="1">
-  <autoFilter ref="B4:C5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Ages" displayName="Ages" ref="B4:C6" totalsRowCount="1">
+  <autoFilter ref="B4:C5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Name" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Age" totalsRowFunction="count"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Age" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Days" displayName="Days" ref="B7:C8" totalsRowShown="0">
-  <autoFilter ref="B7:C8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Days" displayName="Days" ref="B7:C8" totalsRowShown="0">
+  <autoFilter ref="B7:C8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="${days}"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="${days}"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Status" displayName="Status" ref="C12:D14" totalsRowShown="0">
-  <autoFilter ref="C12:D14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Status" displayName="Status" ref="C12:D14" totalsRowShown="0">
+  <autoFilter ref="C12:D14" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Colour"/>
-    <tableColumn id="2" name="Status"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Colour"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -513,28 +538,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="20" thickBot="1">
+    <row r="2" spans="2:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="2:6" ht="16" thickTop="1"/>
-    <row r="4" spans="2:6">
+    <row r="3" spans="2:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -542,7 +567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -550,7 +575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -559,7 +584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -574,7 +599,7 @@
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -582,13 +607,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>103</v>
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
@@ -605,7 +630,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>11</v>
       </c>
@@ -613,7 +638,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
@@ -621,12 +646,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>105</v>
       </c>
@@ -634,7 +659,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="2:10">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="J27" t="s">
         <v>16</v>
       </c>
@@ -645,12 +670,12 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="E7:F7"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <tableParts count="3">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Fix adjustment of definedNames
</commit_message>
<xml_diff>
--- a/test/templates/test-named-tables.xlsx
+++ b/test/templates/test-named-tables.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mitrais\cac\olive-2021\xlsx-template\test\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neuhaeusser\Documents\aws\projects\forks\xlsx-template\test\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC52F1DE-F66C-4F7A-9A91-F3AAAF458473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBCF04F-A457-414D-ADE5-5B887062EA1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
+    <sheet name="Untouched" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="BelowTable">Tables!$B$16</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Tables!$1:$3</definedName>
+    <definedName name="Formula">IF(Tables!$G$7&gt;1,Tables!$G$6,SUM(Untouched!$A$2:$A$6)/COUNT(Untouched!$A$2:$A$6))</definedName>
     <definedName name="Moving">Tables!$E$7</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Tables!$1:$3</definedName>
     <definedName name="RangeBelowTable">Tables!$B$17:$C$17</definedName>
     <definedName name="RangeRightOfTable">Tables!$E$12:$F$12</definedName>
     <definedName name="RightOfTable">Tables!$D$7</definedName>
@@ -42,8 +44,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Named tables</t>
   </si>
@@ -94,6 +118,18 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>some values</t>
+  </si>
+  <si>
+    <t>defined name with formula</t>
+  </si>
+  <si>
+    <t>helper</t>
+  </si>
+  <si>
+    <t>formula</t>
   </si>
 </sst>
 </file>
@@ -155,9 +191,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -167,9 +202,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Prozent" xfId="2" builtinId="5"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift 1" xfId="1" builtinId="16"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -541,25 +576,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="2:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" ht="16" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -567,15 +615,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H5" cm="1">
+        <f t="array" ref="H5">Formula</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -583,8 +635,11 @@
         <f>SUBTOTAL(103,Ages[Age])</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -594,12 +649,15 @@
       <c r="D7">
         <v>101</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>102</v>
       </c>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F7" s="3"/>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -607,14 +665,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="4">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="3">
         <v>103</v>
       </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
+      <c r="C10" s="3"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
@@ -630,7 +688,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>11</v>
       </c>
@@ -638,20 +696,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="1" t="s">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>105</v>
       </c>
@@ -659,16 +717,17 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="J27" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G2:H2"/>
   </mergeCells>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -683,4 +742,49 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D592CE32-ADAB-4276-B787-4607EBD97878}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>